<commit_message>
função de normalização de palavras adicionada
</commit_message>
<xml_diff>
--- a/Kit Kat.xlsx
+++ b/Kit Kat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="465">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1458,6 +1458,9 @@
   </si>
   <si>
     <t>eu amo kit kat meu deus 😍</t>
+  </si>
+  <si>
+    <t>Classificacao</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,6 +1876,9 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -4285,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4298,6 +4304,9 @@
       <c r="A1" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="B1" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
adicionadas as ultimas funções
</commit_message>
<xml_diff>
--- a/Kit Kat.xlsx
+++ b/Kit Kat.xlsx
@@ -1864,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2134,7 +2134,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>